<commit_message>
updating emotions, adding text status
</commit_message>
<xml_diff>
--- a/thesaurii/xlsx/Emotions.xlsx
+++ b/thesaurii/xlsx/Emotions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9000" yWindow="4600" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -609,7 +609,7 @@
   <dimension ref="A1:L76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -617,6 +617,8 @@
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.1640625" customWidth="1"/>
+    <col min="6" max="6" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" x14ac:dyDescent="0.3">
@@ -1676,5 +1678,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>